<commit_message>
Add several Perl scripts for index design. Regenerate v3 files.
</commit_message>
<xml_diff>
--- a/forwardprimer-v3_01.xlsx
+++ b/forwardprimer-v3_01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="60" windowWidth="19176" windowHeight="15528"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="45096" windowHeight="22872"/>
   </bookViews>
   <sheets>
     <sheet name="forwardprimer-v3_01" sheetId="1" r:id="rId1"/>
@@ -28,865 +28,865 @@
     <t>A1</t>
   </si>
   <si>
-    <t>F0001-GATCCAAGTG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGATCCAAGTGTCGTCGGCAGCGTC</t>
+    <t>F0001-TAGAAGCATG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTAGAAGCATGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>A2</t>
   </si>
   <si>
-    <t>F0002-GTAGTGTCCT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGTAGTGTCCTTCGTCGGCAGCGTC</t>
+    <t>F0002-TCGTACTCCT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTCGTACTCCTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>A3</t>
   </si>
   <si>
-    <t>F0003-TTCTTGTGCT</t>
+    <t>F0003-GTCTACTGAC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGTCTACTGACTCGTCGGCAGCGTC</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>F0004-GATGGTCAAG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGATGGTCAAGTCGTCGGCAGCGTC</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>F0005-CTGAAGTCTG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCTGAAGTCTGTCGTCGGCAGCGTC</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>F0006-TTCTTGTGCT</t>
   </si>
   <si>
     <t>AATGATACGGCGACCACCGAGATCTACACTTCTTGTGCTTCGTCGGCAGCGTC</t>
   </si>
   <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>F0004-GTCAACAGAA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGTCAACAGAATCGTCGGCAGCGTC</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>F0005-CCACAGAGTT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACCCACAGAGTTTCGTCGGCAGCGTC</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>F0006-ACTTGACAGA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACTTGACAGATCGTCGGCAGCGTC</t>
-  </si>
-  <si>
     <t>A7</t>
   </si>
   <si>
-    <t>F0007-ATCCTGAGTC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACATCCTGAGTCTCGTCGGCAGCGTC</t>
+    <t>F0007-TTCCATGTGC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTTCCATGTGCTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>A8</t>
   </si>
   <si>
-    <t>F0008-AGCAGTGTTG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAGCAGTGTTGTCGTCGGCAGCGTC</t>
+    <t>F0008-CATCAGTTGC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCATCAGTTGCTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>A9</t>
   </si>
   <si>
-    <t>F0009-GCTACGTTGT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGCTACGTTGTTCGTCGGCAGCGTC</t>
+    <t>F0009-AGACGTAGAC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAGACGTAGACTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>A10</t>
   </si>
   <si>
-    <t>F0010-ACAGGACGTT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACAGGACGTTTCGTCGGCAGCGTC</t>
+    <t>F0010-TGCTTCTGTG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTGCTTCTGTGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>A11</t>
   </si>
   <si>
-    <t>F0011-CAACTAGGTC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACCAACTAGGTCTCGTCGGCAGCGTC</t>
+    <t>F0011-TCTCCAACAG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTCTCCAACAGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>A12</t>
   </si>
   <si>
-    <t>F0012-CGAGTCATCT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACCGAGTCATCTTCGTCGGCAGCGTC</t>
+    <t>F0012-GAACGATCAT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGAACGATCATTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>B1</t>
   </si>
   <si>
-    <t>F0013-TCGTGGTCTA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTCGTGGTCTATCGTCGGCAGCGTC</t>
+    <t>F0013-TGGAGAACAT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTGGAGAACATTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>B2</t>
   </si>
   <si>
-    <t>F0014-GCTGTAGTGT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGCTGTAGTGTTCGTCGGCAGCGTC</t>
+    <t>F0014-CATGTCTACC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCATGTCTACCTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>B3</t>
   </si>
   <si>
-    <t>F0015-CAACGTCAGA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACCAACGTCAGATCGTCGGCAGCGTC</t>
+    <t>F0015-ATCAGCTCGA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACATCAGCTCGATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>B4</t>
   </si>
   <si>
-    <t>F0016-TGGTGATGAC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTGGTGATGACTCGTCGGCAGCGTC</t>
+    <t>F0016-ATCCAAGAGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACATCCAAGAGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>B5</t>
   </si>
   <si>
-    <t>F0017-TTGAGGTCAT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTTGAGGTCATTCGTCGGCAGCGTC</t>
+    <t>F0017-TGCTGAACGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTGCTGAACGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>B6</t>
   </si>
   <si>
-    <t>F0018-AACACTTCTC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAACACTTCTCTCGTCGGCAGCGTC</t>
+    <t>F0018-TCTCACTTGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTCTCACTTGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>B7</t>
   </si>
   <si>
-    <t>F0019-GAACTCAACC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGAACTCAACCTCGTCGGCAGCGTC</t>
+    <t>F0019-GCATGTCGTA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGCATGTCGTATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>B8</t>
   </si>
   <si>
-    <t>F0020-TGAGCTGATG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTGAGCTGATGTCGTCGGCAGCGTC</t>
+    <t>F0020-TCTCACTGAC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTCTCACTGACTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>B9</t>
   </si>
   <si>
-    <t>F0021-AGACTACGAA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAGACTACGAATCGTCGGCAGCGTC</t>
+    <t>F0021-GCTTCAGAGA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGCTTCAGAGATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>B10</t>
   </si>
   <si>
-    <t>F0022-CTCATGAGTT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACCTCATGAGTTTCGTCGGCAGCGTC</t>
+    <t>F0022-AGTGTCTAGG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAGTGTCTAGGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>B11</t>
   </si>
   <si>
-    <t>F0023-AAGTGACACG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAAGTGACACGTCGTCGGCAGCGTC</t>
+    <t>F0023-CTAGCAGTAC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCTAGCAGTACTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>B12</t>
   </si>
   <si>
-    <t>F0024-CTGACATCCT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACCTGACATCCTTCGTCGGCAGCGTC</t>
+    <t>F0024-TACCATGCTA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTACCATGCTATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>C1</t>
   </si>
   <si>
-    <t>F0025-AACACGACTT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAACACGACTTTCGTCGGCAGCGTC</t>
+    <t>F0025-TAGTCCTAGC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTAGTCCTAGCTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>C2</t>
   </si>
   <si>
-    <t>F0026-GACTTCTGAG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGACTTCTGAGTCGTCGGCAGCGTC</t>
+    <t>F0026-GTAGTGATGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGTAGTGATGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>C3</t>
   </si>
   <si>
-    <t>F0027-GAACATGTGA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGAACATGTGATCGTCGGCAGCGTC</t>
+    <t>F0027-GCTGATCTAG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGCTGATCTAGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>C4</t>
   </si>
   <si>
-    <t>F0028-GTGACTGCAA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGTGACTGCAATCGTCGGCAGCGTC</t>
+    <t>F0028-CTTGCTGTTC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCTTGCTGTTCTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>C5</t>
   </si>
   <si>
-    <t>F0029-ACCATGCAAC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACCATGCAACTCGTCGGCAGCGTC</t>
+    <t>F0029-AGTTCCTACA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAGTTCCTACATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>C6</t>
   </si>
   <si>
-    <t>F0030-AGAGTGCTTG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAGAGTGCTTGTCGTCGGCAGCGTC</t>
+    <t>F0030-CACAGCACAT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCACAGCACATTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>C7</t>
   </si>
   <si>
-    <t>F0031-GTACTCCTTG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGTACTCCTTGTCGTCGGCAGCGTC</t>
+    <t>F0031-AACACCTTGC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAACACCTTGCTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>C8</t>
   </si>
   <si>
-    <t>F0032-TGTGAAGAGT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTGTGAAGAGTTCGTCGGCAGCGTC</t>
+    <t>F0032-GATCGAACCA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGATCGAACCATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>C9</t>
   </si>
   <si>
-    <t>F0033-GACAGGTGAT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGACAGGTGATTCGTCGGCAGCGTC</t>
+    <t>F0033-AGTCACCTAC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAGTCACCTACTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>C10</t>
   </si>
   <si>
-    <t>F0034-AACATCAGCT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAACATCAGCTTCGTCGGCAGCGTC</t>
+    <t>F0034-GTGCATGGAT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGTGCATGGATTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>C11</t>
   </si>
   <si>
-    <t>F0035-TCATGGTGTT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTCATGGTGTTTCGTCGGCAGCGTC</t>
+    <t>F0035-CTTCAGTAGA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCTTCAGTAGATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>C12</t>
   </si>
   <si>
-    <t>F0036-AGGATCTCCT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAGGATCTCCTTCGTCGGCAGCGTC</t>
+    <t>F0036-GACTGTAGTG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGACTGTAGTGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>D1</t>
   </si>
   <si>
-    <t>F0037-ACTCAGGAAG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACTCAGGAAGTCGTCGGCAGCGTC</t>
+    <t>F0037-TCCTGTACTG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTCCTGTACTGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>D2</t>
   </si>
   <si>
-    <t>F0038-CTCTTCGTGA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACCTCTTCGTGATCGTCGGCAGCGTC</t>
+    <t>F0038-CTCTCTACAC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCTCTCTACACTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>D3</t>
   </si>
   <si>
-    <t>F0039-TCATCCACAA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTCATCCACAATCGTCGGCAGCGTC</t>
+    <t>F0039-ACACCACGAT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACACACCACGATTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>D4</t>
   </si>
   <si>
-    <t>F0040-TCTTGTCGAG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTCTTGTCGAGTCGTCGGCAGCGTC</t>
+    <t>F0040-ATGACTCCTC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACATGACTCCTCTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>D5</t>
   </si>
   <si>
-    <t>F0041-GGTGAAGTGA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGGTGAAGTGATCGTCGGCAGCGTC</t>
+    <t>F0041-CATGGAAGAT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCATGGAAGATTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>D6</t>
   </si>
   <si>
-    <t>F0042-TCTACGTCAG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTCTACGTCAGTCGTCGGCAGCGTC</t>
+    <t>F0042-CCTTCTCACT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCCTTCTCACTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>D7</t>
   </si>
   <si>
-    <t>F0043-CATCGTGATC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACCATCGTGATCTCGTCGGCAGCGTC</t>
+    <t>F0043-ACATGCAGGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACACATGCAGGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>D8</t>
   </si>
   <si>
-    <t>F0044-AAGAGTAGCA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAAGAGTAGCATCGTCGGCAGCGTC</t>
+    <t>F0044-ACACATCGTT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACACACATCGTTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>D9</t>
   </si>
   <si>
-    <t>F0045-TTCAGCTGCT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTTCAGCTGCTTCGTCGGCAGCGTC</t>
+    <t>F0045-TCAAGCACAG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTCAAGCACAGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>D10</t>
   </si>
   <si>
-    <t>F0046-ACTCCAACCA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACTCCAACCATCGTCGGCAGCGTC</t>
+    <t>F0046-CATGACGAGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCATGACGAGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>D11</t>
   </si>
   <si>
-    <t>F0047-ACAACAGTGC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACAACAGTGCTCGTCGGCAGCGTC</t>
+    <t>F0047-GCAGACAGTA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGCAGACAGTATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>D12</t>
   </si>
   <si>
-    <t>F0048-CAGGTGACTA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACCAGGTGACTATCGTCGGCAGCGTC</t>
+    <t>F0048-TTGTGAGAAG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTTGTGAGAAGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>E1</t>
   </si>
   <si>
-    <t>F0049-AACTCGTGTA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAACTCGTGTATCGTCGGCAGCGTC</t>
+    <t>F0049-ACCATGTAGG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACACCATGTAGGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>E2</t>
   </si>
   <si>
-    <t>F0050-GTTGGAGCAT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGTTGGAGCATTCGTCGGCAGCGTC</t>
+    <t>F0050-TCAGCAGAAC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTCAGCAGAACTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>E3</t>
   </si>
   <si>
-    <t>F0051-GGAGTACCAT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGGAGTACCATTCGTCGGCAGCGTC</t>
+    <t>F0051-ACATCCTCCT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACACATCCTCCTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>E4</t>
   </si>
   <si>
-    <t>F0052-AACTGGAGCA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAACTGGAGCATCGTCGGCAGCGTC</t>
+    <t>F0052-AAGGACAAGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAAGGACAAGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>E5</t>
   </si>
   <si>
-    <t>F0053-GGACTTCAGA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGGACTTCAGATCGTCGGCAGCGTC</t>
+    <t>F0053-GAGGTGTGAT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGAGGTGTGATTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>E6</t>
   </si>
   <si>
-    <t>F0054-ACCATGAGTG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACCATGAGTGTCGTCGGCAGCGTC</t>
+    <t>F0054-AGATGACTTG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAGATGACTTGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>E7</t>
   </si>
   <si>
-    <t>F0055-GAACTCGTAC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGAACTCGTACTCGTCGGCAGCGTC</t>
+    <t>F0055-TTGCTAGATC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTTGCTAGATCTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>E8</t>
   </si>
   <si>
-    <t>F0056-ACGTTGTGAA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACGTTGTGAATCGTCGGCAGCGTC</t>
+    <t>F0056-TCTGCAGGTT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTCTGCAGGTTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>E9</t>
   </si>
   <si>
-    <t>F0057-TTGCACACTC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTTGCACACTCTCGTCGGCAGCGTC</t>
+    <t>F0057-AACGAGGAGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAACGAGGAGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>E10</t>
   </si>
   <si>
-    <t>F0058-AAGAGACCAG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAAGAGACCAGTCGTCGGCAGCGTC</t>
+    <t>F0058-TGAGGACAAG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTGAGGACAAGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>E11</t>
   </si>
   <si>
-    <t>F0059-TCTACGTAGC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTCTACGTAGCTCGTCGGCAGCGTC</t>
+    <t>F0059-GTTCTCTCCT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGTTCTCTCCTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>E12</t>
   </si>
   <si>
-    <t>F0060-AACACAGACT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAACACAGACTTCGTCGGCAGCGTC</t>
+    <t>F0060-TCGAGATCTG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTCGAGATCTGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>F1</t>
   </si>
   <si>
-    <t>F0061-TTCTCCAAGT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTTCTCCAAGTTCGTCGGCAGCGTC</t>
+    <t>F0061-AGGTGAAGAG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAGGTGAAGAGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>F2</t>
   </si>
   <si>
-    <t>F0062-ACACTCACTA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACACTCACTATCGTCGGCAGCGTC</t>
+    <t>F0062-AAGTCGACCA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAAGTCGACCATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>F3</t>
   </si>
   <si>
-    <t>F0063-GGACACTGTT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGGACACTGTTTCGTCGGCAGCGTC</t>
+    <t>F0063-TTCCAAGCAT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTTCCAAGCATTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>F4</t>
   </si>
   <si>
-    <t>F0064-CAACGTTCAC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACCAACGTTCACTCGTCGGCAGCGTC</t>
+    <t>F0064-AACCAGTACA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAACCAGTACATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>F5</t>
   </si>
   <si>
-    <t>F0065-ACTGTTGCAT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACTGTTGCATTCGTCGGCAGCGTC</t>
+    <t>F0065-ACCTTGTCTA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACACCTTGTCTATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>F6</t>
   </si>
   <si>
-    <t>F0066-ACGTAGACTA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACGTAGACTATCGTCGGCAGCGTC</t>
+    <t>F0066-TCACAGGTTG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTCACAGGTTGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>F7</t>
   </si>
   <si>
-    <t>F0067-ATGCAAGACC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACATGCAAGACCTCGTCGGCAGCGTC</t>
+    <t>F0067-AACTACGTGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAACTACGTGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>F8</t>
   </si>
   <si>
-    <t>F0068-TCACAGAAGG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTCACAGAAGGTCGTCGGCAGCGTC</t>
+    <t>F0068-CGTCGTTGTA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCGTCGTTGTATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>F9</t>
   </si>
   <si>
-    <t>F0069-TCAGTAGAGA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTCAGTAGAGATCGTCGGCAGCGTC</t>
+    <t>F0069-CAGTAGGTGA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCAGTAGGTGATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>F10</t>
   </si>
   <si>
-    <t>F0070-TGACTGGAAC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTGACTGGAACTCGTCGGCAGCGTC</t>
+    <t>F0070-ACAGTGCAGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACACAGTGCAGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>F11</t>
   </si>
   <si>
-    <t>F0071-AACGTCCTTG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAACGTCCTTGTCGTCGGCAGCGTC</t>
+    <t>F0071-ACTCGAGTTG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACACTCGAGTTGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>F12</t>
   </si>
   <si>
-    <t>F0072-GCTTCTGAAC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGCTTCTGAACTCGTCGGCAGCGTC</t>
+    <t>F0072-ATCACACGTG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACATCACACGTGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>G1</t>
   </si>
   <si>
-    <t>F0073-CGATCGAGAA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACCGATCGAGAATCGTCGGCAGCGTC</t>
+    <t>F0073-GTCTGGTTCT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGTCTGGTTCTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>G2</t>
   </si>
   <si>
-    <t>F0074-TGGTTCGAAG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTGGTTCGAAGTCGTCGGCAGCGTC</t>
+    <t>F0074-AAGCACACAA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAAGCACACAATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>G3</t>
   </si>
   <si>
-    <t>F0075-TCTACCATCA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTCTACCATCATCGTCGGCAGCGTC</t>
+    <t>F0075-TACGACCATC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTACGACCATCTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>G4</t>
   </si>
   <si>
-    <t>F0076-TACTAGTCGA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTACTAGTCGATCGTCGGCAGCGTC</t>
+    <t>F0076-GTGATCCTTC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGTGATCCTTCTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>G5</t>
   </si>
   <si>
-    <t>F0077-AACGTTGGTG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAACGTTGGTGTCGTCGGCAGCGTC</t>
+    <t>F0077-CGTTCCATGA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCGTTCCATGATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>G6</t>
   </si>
   <si>
-    <t>F0078-TGGATCAACG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTGGATCAACGTCGTCGGCAGCGTC</t>
+    <t>F0078-GAACTCTGCT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGAACTCTGCTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>G7</t>
   </si>
   <si>
-    <t>F0079-TAGTGAACTG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTAGTGAACTGTCGTCGGCAGCGTC</t>
+    <t>F0079-GAGTGAGATC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGAGTGAGATCTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>G8</t>
   </si>
   <si>
-    <t>F0080-AGTCTCTCAA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAGTCTCTCAATCGTCGGCAGCGTC</t>
+    <t>F0080-ACAGAGTGGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACACAGAGTGGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>G9</t>
   </si>
   <si>
-    <t>F0081-TACTTGAGAC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTACTTGAGACTCGTCGGCAGCGTC</t>
+    <t>F0081-AACCTGAGAA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACAACCTGAGAATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>G10</t>
   </si>
   <si>
-    <t>F0082-AGTCAACAGC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAGTCAACAGCTCGTCGGCAGCGTC</t>
+    <t>F0082-ACAGGTACAC</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACACAGGTACACTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>G11</t>
   </si>
   <si>
-    <t>F0083-GTTGTTGACA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGTTGTTGACATCGTCGGCAGCGTC</t>
+    <t>F0083-CTGAACAGCT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCTGAACAGCTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>G12</t>
   </si>
   <si>
-    <t>F0084-AGTCAAGCAG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAGTCAAGCAGTCGTCGGCAGCGTC</t>
+    <t>F0084-GTAGACAACG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGTAGACAACGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>H1</t>
   </si>
   <si>
-    <t>F0085-AGTTCAGCTT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAGTTCAGCTTTCGTCGGCAGCGTC</t>
+    <t>F0085-CCATGTGTGA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCCATGTGTGATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>H2</t>
   </si>
   <si>
-    <t>F0086-TACGAAGCTT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTACGAAGCTTTCGTCGGCAGCGTC</t>
+    <t>F0086-TGGTCGTCTT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTGGTCGTCTTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>H3</t>
   </si>
   <si>
-    <t>F0087-ACCTTGTCTA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACCTTGTCTATCGTCGGCAGCGTC</t>
+    <t>F0087-GATGGTTCGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGATGGTTCGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>H4</t>
   </si>
   <si>
-    <t>F0088-TGACACATGC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTGACACATGCTCGTCGGCAGCGTC</t>
+    <t>F0088-CAGACATCTA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCAGACATCTATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>H5</t>
   </si>
   <si>
-    <t>F0089-GTCAGTTGTA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGTCAGTTGTATCGTCGGCAGCGTC</t>
+    <t>F0089-CCAGACAAGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCCAGACAAGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>H6</t>
   </si>
   <si>
-    <t>F0090-GTGTCTTCAT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACGTGTCTTCATTCGTCGGCAGCGTC</t>
+    <t>F0090-TACTCTGTGG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTACTCTGTGGTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>H7</t>
   </si>
   <si>
-    <t>F0091-ACAGAAGCTG</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACAGAAGCTGTCGTCGGCAGCGTC</t>
+    <t>F0091-ATGTGTAGGT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACATGTGTAGGTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>H8</t>
   </si>
   <si>
-    <t>F0092-AACGTAGCTA</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAACGTAGCTATCGTCGGCAGCGTC</t>
+    <t>F0092-CGATGACCTT</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCGATGACCTTTCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>H9</t>
   </si>
   <si>
-    <t>F0093-AGGTCAACTC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACAGGTCAACTCTCGTCGGCAGCGTC</t>
+    <t>F0093-GTCAAGACTA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGTCAAGACTATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>H10</t>
   </si>
   <si>
-    <t>F0094-ACATCTCCTC</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACACATCTCCTCTCGTCGGCAGCGTC</t>
+    <t>F0094-CTGCACTTCA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACCTGCACTTCATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>H11</t>
   </si>
   <si>
-    <t>F0095-TAGTGTCCAT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTAGTGTCCATTCGTCGGCAGCGTC</t>
+    <t>F0095-GAACCTCTCA</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACGAACCTCTCATCGTCGGCAGCGTC</t>
   </si>
   <si>
     <t>H12</t>
   </si>
   <si>
-    <t>F0096-TACACTGGTT</t>
-  </si>
-  <si>
-    <t>AATGATACGGCGACCACCGAGATCTACACTACACTGGTTTCGTCGGCAGCGTC</t>
+    <t>F0096-TGGTCATCAG</t>
+  </si>
+  <si>
+    <t>AATGATACGGCGACCACCGAGATCTACACTGGTCATCAGTCGTCGGCAGCGTC</t>
   </si>
 </sst>
 </file>

</xml_diff>